<commit_message>
Responsibility allocation matrix update
</commit_message>
<xml_diff>
--- a/docs/ResponsibilityAssignmentMatrix.xlsx
+++ b/docs/ResponsibilityAssignmentMatrix.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S533987\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S534118\Documents\GitHub\PuMpup\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E058E4CB-0CE9-4181-B884-3907F2204DE6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{521E55D5-9523-4144-B61D-CB554A02B6CB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B9EC7B93-AE71-406D-ADAE-EDBDCA600810}"/>
   </bookViews>
@@ -23,7 +23,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="35">
   <si>
     <r>
       <t xml:space="preserve"> 
@@ -303,9 +302,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -316,6 +312,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -661,9 +660,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDE7AC00-27E9-404B-841E-C18E919B6BF8}">
   <dimension ref="A1:AB35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="76" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -798,7 +797,7 @@
     <col min="16130" max="16155" width="3.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="159.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -831,381 +830,461 @@
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6"/>
-      <c r="S2" s="6"/>
-      <c r="T2" s="6"/>
-      <c r="U2" s="6"/>
-      <c r="V2" s="6"/>
-      <c r="W2" s="6"/>
-      <c r="X2" s="6"/>
-      <c r="Y2" s="6"/>
-      <c r="Z2" s="6"/>
-      <c r="AA2" s="6"/>
-      <c r="AB2" s="6"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
+      <c r="T2" s="5"/>
+      <c r="U2" s="5"/>
+      <c r="V2" s="5"/>
+      <c r="W2" s="5"/>
+      <c r="X2" s="5"/>
+      <c r="Y2" s="5"/>
+      <c r="Z2" s="5"/>
+      <c r="AA2" s="5"/>
+      <c r="AB2" s="5"/>
     </row>
     <row r="3" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
     </row>
     <row r="4" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
     </row>
     <row r="5" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-    </row>
-    <row r="6" spans="1:28" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+    </row>
+    <row r="6" spans="1:28" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
     </row>
     <row r="7" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
-      <c r="N7" s="6"/>
-      <c r="O7" s="6"/>
-      <c r="P7" s="6"/>
-      <c r="Q7" s="6"/>
-      <c r="R7" s="6"/>
-      <c r="S7" s="6"/>
-      <c r="T7" s="6"/>
-      <c r="U7" s="6"/>
-      <c r="V7" s="6"/>
-      <c r="W7" s="6"/>
-      <c r="X7" s="6"/>
-      <c r="Y7" s="6"/>
-      <c r="Z7" s="6"/>
-      <c r="AA7" s="6"/>
+      <c r="B7" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="5"/>
+      <c r="R7" s="5"/>
+      <c r="S7" s="5"/>
+      <c r="T7" s="5"/>
+      <c r="U7" s="5"/>
+      <c r="V7" s="5"/>
+      <c r="W7" s="5"/>
+      <c r="X7" s="5"/>
+      <c r="Y7" s="5"/>
+      <c r="Z7" s="5"/>
+      <c r="AA7" s="5"/>
     </row>
     <row r="8" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="6"/>
-      <c r="O8" s="6"/>
-      <c r="P8" s="6"/>
-      <c r="Q8" s="6"/>
-      <c r="R8" s="6"/>
-      <c r="S8" s="6"/>
-      <c r="T8" s="6"/>
-      <c r="U8" s="6"/>
-      <c r="V8" s="6"/>
-      <c r="W8" s="6"/>
-      <c r="X8" s="6"/>
-      <c r="Y8" s="6"/>
-      <c r="Z8" s="6"/>
-      <c r="AA8" s="6"/>
-    </row>
-    <row r="9" spans="1:28" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="5"/>
+      <c r="S8" s="5"/>
+      <c r="T8" s="5"/>
+      <c r="U8" s="5"/>
+      <c r="V8" s="5"/>
+      <c r="W8" s="5"/>
+      <c r="X8" s="5"/>
+      <c r="Y8" s="5"/>
+      <c r="Z8" s="5"/>
+      <c r="AA8" s="5"/>
+    </row>
+    <row r="9" spans="1:28" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
     </row>
     <row r="10" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="6"/>
-      <c r="O10" s="6"/>
-      <c r="P10" s="6"/>
-      <c r="Q10" s="6"/>
-      <c r="R10" s="6"/>
-      <c r="S10" s="6"/>
-      <c r="T10" s="6"/>
-      <c r="U10" s="6"/>
-      <c r="V10" s="6"/>
-      <c r="W10" s="6"/>
-      <c r="X10" s="6"/>
-      <c r="Y10" s="6"/>
-      <c r="Z10" s="6"/>
-      <c r="AA10" s="6"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="5"/>
+      <c r="R10" s="5"/>
+      <c r="S10" s="5"/>
+      <c r="T10" s="5"/>
+      <c r="U10" s="5"/>
+      <c r="V10" s="5"/>
+      <c r="W10" s="5"/>
+      <c r="X10" s="5"/>
+      <c r="Y10" s="5"/>
+      <c r="Z10" s="5"/>
+      <c r="AA10" s="5"/>
     </row>
     <row r="11" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
-      <c r="N11" s="6"/>
-      <c r="O11" s="6"/>
-      <c r="P11" s="6"/>
-      <c r="Q11" s="6"/>
-      <c r="R11" s="6"/>
-      <c r="S11" s="6"/>
-      <c r="T11" s="6"/>
-      <c r="U11" s="6"/>
-      <c r="V11" s="6"/>
-      <c r="W11" s="6"/>
-      <c r="X11" s="6"/>
-      <c r="Y11" s="6"/>
-      <c r="Z11" s="6"/>
-      <c r="AA11" s="6"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="5"/>
+      <c r="R11" s="5"/>
+      <c r="S11" s="5"/>
+      <c r="T11" s="5"/>
+      <c r="U11" s="5"/>
+      <c r="V11" s="5"/>
+      <c r="W11" s="5"/>
+      <c r="X11" s="5"/>
+      <c r="Y11" s="5"/>
+      <c r="Z11" s="5"/>
+      <c r="AA11" s="5"/>
     </row>
     <row r="12" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
-      <c r="N12" s="6"/>
-      <c r="O12" s="6"/>
-      <c r="P12" s="6"/>
-      <c r="Q12" s="6"/>
-      <c r="R12" s="6"/>
-      <c r="S12" s="6"/>
-      <c r="T12" s="6"/>
-      <c r="U12" s="6"/>
-      <c r="V12" s="6"/>
-      <c r="W12" s="6"/>
-      <c r="X12" s="6"/>
-      <c r="Y12" s="6"/>
-      <c r="Z12" s="6"/>
-      <c r="AA12" s="6"/>
-    </row>
-    <row r="13" spans="1:28" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="4"/>
+      <c r="C12" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
+      <c r="P12" s="5"/>
+      <c r="Q12" s="5"/>
+      <c r="R12" s="5"/>
+      <c r="S12" s="5"/>
+      <c r="T12" s="5"/>
+      <c r="U12" s="5"/>
+      <c r="V12" s="5"/>
+      <c r="W12" s="5"/>
+      <c r="X12" s="5"/>
+      <c r="Y12" s="5"/>
+      <c r="Z12" s="5"/>
+      <c r="AA12" s="5"/>
+    </row>
+    <row r="13" spans="1:28" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
     </row>
     <row r="14" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
     </row>
     <row r="15" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
     </row>
     <row r="16" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
     </row>
     <row r="17" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
     </row>
     <row r="18" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="19" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="20" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
+      <c r="A20" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
+      <c r="B20" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="21" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="24" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="7" t="s">
+      <c r="A28" s="6" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="7" t="s">
+      <c r="A29" s="6" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="30" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="7"/>
+      <c r="A30" s="6"/>
     </row>
     <row r="31" spans="1:9" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">

</xml_diff>